<commit_message>
afino costos y cargo datos de otros autores
</commit_message>
<xml_diff>
--- a/analisis/resultados/renta_hidrocarburos_total.xlsx
+++ b/analisis/resultados/renta_hidrocarburos_total.xlsx
@@ -359,7 +359,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U111"/>
+  <dimension ref="A1:V111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,20 +453,25 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>proporcion_subsidios</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>renta_pv</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>renta_pbi</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>renta_usd_tcc</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>renta_usd_tcp</t>
         </is>
@@ -1684,15 +1689,18 @@
         <v>-54.99641340446073</v>
       </c>
       <c r="R53">
+        <v>-0</v>
+      </c>
+      <c r="S53">
         <v>-3.371355160570678e-005</v>
       </c>
-      <c r="S53">
+      <c r="T53">
         <v>-2.001641548463958e-005</v>
       </c>
-      <c r="T53">
+      <c r="U53">
         <v>-0.1831563094002225</v>
       </c>
-      <c r="U53">
+      <c r="V53">
         <v>-0.1926923392047417</v>
       </c>
     </row>
@@ -1753,15 +1761,18 @@
         <v>-8701.736785914423</v>
       </c>
       <c r="R54">
+        <v>-0</v>
+      </c>
+      <c r="S54">
         <v>-0.00490116455846466</v>
       </c>
-      <c r="S54">
+      <c r="T54">
         <v>-0.003246633956799652</v>
       </c>
-      <c r="T54">
+      <c r="U54">
         <v>-30.46640141229396</v>
       </c>
-      <c r="U54">
+      <c r="V54">
         <v>-30.93416599986339</v>
       </c>
     </row>
@@ -1822,15 +1833,18 @@
         <v>18831.1379047894</v>
       </c>
       <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
         <v>0.009387462039342754</v>
       </c>
-      <c r="S55">
+      <c r="T55">
         <v>0.006279126316546143</v>
       </c>
-      <c r="T55">
+      <c r="U55">
         <v>79.38908759317143</v>
       </c>
-      <c r="U55">
+      <c r="V55">
         <v>70.13177669489221</v>
       </c>
     </row>
@@ -1891,15 +1905,18 @@
         <v>26818.11055331316</v>
       </c>
       <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="S56">
         <v>0.01311455921533785</v>
       </c>
-      <c r="S56">
+      <c r="T56">
         <v>0.008075330112415598</v>
       </c>
-      <c r="T56">
+      <c r="U56">
         <v>122.0245676032575</v>
       </c>
-      <c r="U56">
+      <c r="V56">
         <v>106.0268385703013</v>
       </c>
     </row>
@@ -1960,15 +1977,18 @@
         <v>69868.12013213284</v>
       </c>
       <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57">
         <v>0.03760969598195157</v>
       </c>
-      <c r="S57">
+      <c r="T57">
         <v>0.02060507650375207</v>
       </c>
-      <c r="T57">
+      <c r="U57">
         <v>340.2210711936546</v>
       </c>
-      <c r="U57">
+      <c r="V57">
         <v>282.6997534533968</v>
       </c>
     </row>
@@ -2029,15 +2049,18 @@
         <v>-15604.94538613893</v>
       </c>
       <c r="R58">
+        <v>-0</v>
+      </c>
+      <c r="S58">
         <v>-0.007920382262086578</v>
       </c>
-      <c r="S58">
+      <c r="T58">
         <v>-0.004419210277982406</v>
       </c>
-      <c r="T58">
+      <c r="U58">
         <v>-61.40713772884881</v>
       </c>
-      <c r="U58">
+      <c r="V58">
         <v>-61.9424631918772</v>
       </c>
     </row>
@@ -2098,15 +2121,18 @@
         <v>-43405.65941875908</v>
       </c>
       <c r="R59">
+        <v>-0</v>
+      </c>
+      <c r="S59">
         <v>-0.0206275482122956</v>
       </c>
-      <c r="S59">
+      <c r="T59">
         <v>-0.01161731899188562</v>
       </c>
-      <c r="T59">
+      <c r="U59">
         <v>-187.7456225040636</v>
       </c>
-      <c r="U59">
+      <c r="V59">
         <v>-186.2774730564882</v>
       </c>
     </row>
@@ -2167,15 +2193,18 @@
         <v>-15693.82595098616</v>
       </c>
       <c r="R60">
+        <v>-0</v>
+      </c>
+      <c r="S60">
         <v>-0.006217628644225268</v>
       </c>
-      <c r="S60">
+      <c r="T60">
         <v>-0.00381464506326312</v>
       </c>
-      <c r="T60">
+      <c r="U60">
         <v>-73.0257889574867</v>
       </c>
-      <c r="U60">
+      <c r="V60">
         <v>-76.39121877173776</v>
       </c>
     </row>
@@ -2236,15 +2265,18 @@
         <v>17706.47186349012</v>
       </c>
       <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61">
         <v>0.007098685213435086</v>
       </c>
-      <c r="S61">
+      <c r="T61">
         <v>0.004025684052333426</v>
       </c>
-      <c r="T61">
+      <c r="U61">
         <v>86.87662800043736</v>
       </c>
-      <c r="U61">
+      <c r="V61">
         <v>91.7491861434649</v>
       </c>
     </row>
@@ -2305,15 +2337,18 @@
         <v>45326.92438998339</v>
       </c>
       <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
         <v>0.01733566275856285</v>
       </c>
-      <c r="S62">
+      <c r="T62">
         <v>0.009931188188884525</v>
       </c>
-      <c r="T62">
+      <c r="U62">
         <v>246.0919054582391</v>
       </c>
-      <c r="U62">
+      <c r="V62">
         <v>236.704816181236</v>
       </c>
     </row>
@@ -2374,15 +2409,18 @@
         <v>50062.07791078088</v>
       </c>
       <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
         <v>0.01699597030563181</v>
       </c>
-      <c r="S63">
+      <c r="T63">
         <v>0.01074398153796469</v>
       </c>
-      <c r="T63">
+      <c r="U63">
         <v>247.1031229970754</v>
       </c>
-      <c r="U63">
+      <c r="V63">
         <v>265.0485818749373</v>
       </c>
     </row>
@@ -2443,15 +2481,18 @@
         <v>115622.9914012727</v>
       </c>
       <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
         <v>0.03765059566153541</v>
       </c>
-      <c r="S64">
+      <c r="T64">
         <v>0.0239199969330048</v>
       </c>
-      <c r="T64">
+      <c r="U64">
         <v>843.1918139009479</v>
       </c>
-      <c r="U64">
+      <c r="V64">
         <v>643.3731864120398</v>
       </c>
     </row>
@@ -2512,15 +2553,18 @@
         <v>259109.1555272289</v>
       </c>
       <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
         <v>0.08493733560625436</v>
       </c>
-      <c r="S65">
+      <c r="T65">
         <v>0.05085811296677189</v>
       </c>
-      <c r="T65">
+      <c r="U65">
         <v>2347.166517048996</v>
       </c>
-      <c r="U65">
+      <c r="V65">
         <v>1610.853329373624</v>
       </c>
     </row>
@@ -2581,15 +2625,18 @@
         <v>286746.7315102737</v>
       </c>
       <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="S66">
         <v>0.08836640479725051</v>
       </c>
-      <c r="S66">
+      <c r="T66">
         <v>0.05661803308537144</v>
       </c>
-      <c r="T66">
+      <c r="U66">
         <v>2480.931271984809</v>
       </c>
-      <c r="U66">
+      <c r="V66">
         <v>1704.80013323767</v>
       </c>
     </row>
@@ -2650,15 +2697,18 @@
         <v>242731.259495461</v>
       </c>
       <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67">
         <v>0.05465745272872348</v>
       </c>
-      <c r="S67">
+      <c r="T67">
         <v>0.04793278209204568</v>
       </c>
-      <c r="T67">
+      <c r="U67">
         <v>1604.473432618048</v>
       </c>
-      <c r="U67">
+      <c r="V67">
         <v>1466.83071741738</v>
       </c>
     </row>
@@ -2719,15 +2769,18 @@
         <v>259920.0278331693</v>
       </c>
       <c r="R68">
+        <v>0</v>
+      </c>
+      <c r="S68">
         <v>0.05719474854028998</v>
       </c>
-      <c r="S68">
+      <c r="T68">
         <v>0.04824392837165239</v>
       </c>
-      <c r="T68">
+      <c r="U68">
         <v>2142.898649215063</v>
       </c>
-      <c r="U68">
+      <c r="V68">
         <v>1801.450833508913</v>
       </c>
     </row>
@@ -2788,15 +2841,18 @@
         <v>245225.0446025817</v>
       </c>
       <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="S69">
         <v>0.06398088347662721</v>
       </c>
-      <c r="S69">
+      <c r="T69">
         <v>0.04703390170372029</v>
       </c>
-      <c r="T69">
+      <c r="U69">
         <v>2855.552534123657</v>
       </c>
-      <c r="U69">
+      <c r="V69">
         <v>1787.1762318873</v>
       </c>
     </row>
@@ -2857,15 +2913,18 @@
         <v>510375.4368376298</v>
       </c>
       <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70">
         <v>0.1412150162049811</v>
       </c>
-      <c r="S70">
+      <c r="T70">
         <v>0.09154302793316269</v>
       </c>
-      <c r="T70">
+      <c r="U70">
         <v>9300.938015402489</v>
       </c>
-      <c r="U70">
+      <c r="V70">
         <v>4947.705289355234</v>
       </c>
     </row>
@@ -2926,15 +2985,18 @@
         <v>547543.9271528595</v>
       </c>
       <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
         <v>0.1652430786389297</v>
       </c>
-      <c r="S71">
+      <c r="T71">
         <v>0.0966569126849023</v>
       </c>
-      <c r="T71">
+      <c r="U71">
         <v>14340.43747195559</v>
       </c>
-      <c r="U71">
+      <c r="V71">
         <v>6305.321283146856</v>
       </c>
     </row>
@@ -2995,15 +3057,18 @@
         <v>537980.6878373917</v>
       </c>
       <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
         <v>0.1531717343238858</v>
       </c>
-      <c r="S72">
+      <c r="T72">
         <v>0.1007042434762078</v>
       </c>
-      <c r="T72">
+      <c r="U72">
         <v>11955.49467522837</v>
       </c>
-      <c r="U72">
+      <c r="V72">
         <v>6437.540761328651</v>
       </c>
     </row>
@@ -3064,15 +3129,18 @@
         <v>458865.0459114771</v>
       </c>
       <c r="R73">
+        <v>0</v>
+      </c>
+      <c r="S73">
         <v>0.1034816339278332</v>
       </c>
-      <c r="S73">
+      <c r="T73">
         <v>0.08867848284083625</v>
       </c>
-      <c r="T73">
+      <c r="U73">
         <v>5512.564510562405</v>
       </c>
-      <c r="U73">
+      <c r="V73">
         <v>5761.306861343483</v>
       </c>
     </row>
@@ -3133,15 +3201,18 @@
         <v>325492.8194145669</v>
       </c>
       <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74">
         <v>0.07314590436975259</v>
       </c>
-      <c r="S74">
+      <c r="T74">
         <v>0.06042911422018651</v>
       </c>
-      <c r="T74">
+      <c r="U74">
         <v>3559.773297253124</v>
       </c>
-      <c r="U74">
+      <c r="V74">
         <v>4196.992004204276</v>
       </c>
     </row>
@@ -3202,15 +3273,18 @@
         <v>343233.4931722494</v>
       </c>
       <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="S75">
         <v>0.1075600132194063</v>
       </c>
-      <c r="S75">
+      <c r="T75">
         <v>0.0624741104820221</v>
       </c>
-      <c r="T75">
+      <c r="U75">
         <v>4243.122021465213</v>
       </c>
-      <c r="U75">
+      <c r="V75">
         <v>4404.781407327527</v>
       </c>
     </row>
@@ -3271,15 +3345,18 @@
         <v>299648.4146730994</v>
       </c>
       <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="S76">
         <v>0.1110970540370867</v>
       </c>
-      <c r="S76">
+      <c r="T76">
         <v>0.05861631692712807</v>
       </c>
-      <c r="T76">
+      <c r="U76">
         <v>3227.490597111551</v>
       </c>
-      <c r="U76">
+      <c r="V76">
         <v>3606.199145283455</v>
       </c>
     </row>
@@ -3340,15 +3417,18 @@
         <v>185669.4276276004</v>
       </c>
       <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="S77">
         <v>0.07049768278709045</v>
       </c>
-      <c r="S77">
+      <c r="T77">
         <v>0.03379573141938645</v>
       </c>
-      <c r="T77">
+      <c r="U77">
         <v>2421.327461769248</v>
       </c>
-      <c r="U77">
+      <c r="V77">
         <v>2546.968168203092</v>
       </c>
     </row>
@@ -3409,15 +3489,18 @@
         <v>164598.3454081766</v>
       </c>
       <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78">
         <v>0.05597181480600154</v>
       </c>
-      <c r="S78">
+      <c r="T78">
         <v>0.02930907189136686</v>
       </c>
-      <c r="T78">
+      <c r="U78">
         <v>2185.82928650315</v>
       </c>
-      <c r="U78">
+      <c r="V78">
         <v>2243.756777140258</v>
       </c>
     </row>
@@ -3478,15 +3561,18 @@
         <v>62774.45346089987</v>
       </c>
       <c r="R79">
+        <v>0</v>
+      </c>
+      <c r="S79">
         <v>0.01715212223392481</v>
       </c>
-      <c r="S79">
+      <c r="T79">
         <v>0.01140106525867514</v>
       </c>
-      <c r="T79">
+      <c r="U79">
         <v>907.2520266933472</v>
       </c>
-      <c r="U79">
+      <c r="V79">
         <v>809.8220686141972</v>
       </c>
     </row>
@@ -3547,15 +3633,18 @@
         <v>273429.5047645484</v>
       </c>
       <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80">
         <v>0.07880224659487739</v>
       </c>
-      <c r="S80">
+      <c r="T80">
         <v>0.05340255726939454</v>
       </c>
-      <c r="T80">
+      <c r="U80">
         <v>2777.569613528003</v>
       </c>
-      <c r="U80">
+      <c r="V80">
         <v>3650.616537329649</v>
       </c>
     </row>
@@ -3616,15 +3705,18 @@
         <v>277770.6679692788</v>
       </c>
       <c r="R81">
+        <v>0</v>
+      </c>
+      <c r="S81">
         <v>0.1092787565309399</v>
       </c>
-      <c r="S81">
+      <c r="T81">
         <v>0.05498600898736616</v>
       </c>
-      <c r="T81">
+      <c r="U81">
         <v>5977.043248534821</v>
       </c>
-      <c r="U81">
+      <c r="V81">
         <v>3626.633243641759</v>
       </c>
     </row>
@@ -3685,15 +3777,18 @@
         <v>309033.38563813</v>
       </c>
       <c r="R82">
+        <v>0</v>
+      </c>
+      <c r="S82">
         <v>0.1096939024853556</v>
       </c>
-      <c r="S82">
+      <c r="T82">
         <v>0.05536145107376057</v>
       </c>
-      <c r="T82">
+      <c r="U82">
         <v>8538.322046671185</v>
       </c>
-      <c r="U82">
+      <c r="V82">
         <v>4742.198020551375</v>
       </c>
     </row>
@@ -3754,15 +3849,18 @@
         <v>213029.7333637712</v>
       </c>
       <c r="R83">
+        <v>0</v>
+      </c>
+      <c r="S83">
         <v>0.07789608161418613</v>
       </c>
-      <c r="S83">
+      <c r="T83">
         <v>0.03459944482520393</v>
       </c>
-      <c r="T83">
+      <c r="U83">
         <v>7054.36784993315</v>
       </c>
-      <c r="U83">
+      <c r="V83">
         <v>3631.216113686618</v>
       </c>
     </row>
@@ -3823,15 +3921,18 @@
         <v>119963.1095863722</v>
       </c>
       <c r="R84">
+        <v>0</v>
+      </c>
+      <c r="S84">
         <v>0.05205100996930267</v>
       </c>
-      <c r="S84">
+      <c r="T84">
         <v>0.01839335165673722</v>
       </c>
-      <c r="T84">
+      <c r="U84">
         <v>4394.059875923607</v>
       </c>
-      <c r="U84">
+      <c r="V84">
         <v>2192.521169112788</v>
       </c>
     </row>
@@ -3892,15 +3993,18 @@
         <v>103852.3461471902</v>
       </c>
       <c r="R85">
+        <v>0</v>
+      </c>
+      <c r="S85">
         <v>0.03642098529904814</v>
       </c>
-      <c r="S85">
+      <c r="T85">
         <v>0.01512840083516856</v>
       </c>
-      <c r="T85">
+      <c r="U85">
         <v>3923.221783282834</v>
       </c>
-      <c r="U85">
+      <c r="V85">
         <v>2039.553879271167</v>
       </c>
     </row>
@@ -3961,15 +4065,18 @@
         <v>129975.935649184</v>
       </c>
       <c r="R86">
+        <v>0</v>
+      </c>
+      <c r="S86">
         <v>0.0465368118990789</v>
       </c>
-      <c r="S86">
+      <c r="T86">
         <v>0.01938601463623986</v>
       </c>
-      <c r="T86">
+      <c r="U86">
         <v>5127.131714348807</v>
       </c>
-      <c r="U86">
+      <c r="V86">
         <v>2515.947208563899</v>
       </c>
     </row>
@@ -4030,15 +4137,18 @@
         <v>144771.6243869278</v>
       </c>
       <c r="R87">
+        <v>0</v>
+      </c>
+      <c r="S87">
         <v>0.0437291528300675</v>
       </c>
-      <c r="S87">
+      <c r="T87">
         <v>0.02035523725927014</v>
       </c>
-      <c r="T87">
+      <c r="U87">
         <v>5662.4679583731</v>
       </c>
-      <c r="U87">
+      <c r="V87">
         <v>3047.868804120387</v>
       </c>
     </row>
@@ -4099,15 +4209,18 @@
         <v>123843.9200951573</v>
       </c>
       <c r="R88">
+        <v>0</v>
+      </c>
+      <c r="S88">
         <v>0.03286386006437828</v>
       </c>
-      <c r="S88">
+      <c r="T88">
         <v>0.0161485199656993</v>
       </c>
-      <c r="T88">
+      <c r="U88">
         <v>4869.525375534809</v>
       </c>
-      <c r="U88">
+      <c r="V88">
         <v>2753.643396760613</v>
       </c>
     </row>
@@ -4168,15 +4281,18 @@
         <v>71750.93678234912</v>
       </c>
       <c r="R89">
+        <v>0</v>
+      </c>
+      <c r="S89">
         <v>0.01883044223211534</v>
       </c>
-      <c r="S89">
+      <c r="T89">
         <v>0.009182718834991444</v>
       </c>
-      <c r="T89">
+      <c r="U89">
         <v>2847.323773483658</v>
       </c>
-      <c r="U89">
+      <c r="V89">
         <v>1614.181567306336</v>
       </c>
     </row>
@@ -4237,15 +4353,18 @@
         <v>102053.8203577462</v>
       </c>
       <c r="R90">
+        <v>0</v>
+      </c>
+      <c r="S90">
         <v>0.02862358017611458</v>
       </c>
-      <c r="S90">
+      <c r="T90">
         <v>0.013511708507632</v>
       </c>
-      <c r="T90">
+      <c r="U90">
         <v>4002.597067099508</v>
       </c>
-      <c r="U90">
+      <c r="V90">
         <v>2198.507270600949</v>
       </c>
     </row>
@@ -4306,15 +4425,18 @@
         <v>207172.251629181</v>
       </c>
       <c r="R91">
+        <v>0</v>
+      </c>
+      <c r="S91">
         <v>0.05540893818235265</v>
       </c>
-      <c r="S91">
+      <c r="T91">
         <v>0.02690924495316437</v>
       </c>
-      <c r="T91">
+      <c r="U91">
         <v>8049.120917811913</v>
       </c>
-      <c r="U91">
+      <c r="V91">
         <v>4569.419960096972</v>
       </c>
     </row>
@@ -4375,15 +4497,18 @@
         <v>162716.3066240641</v>
       </c>
       <c r="R92">
+        <v>0</v>
+      </c>
+      <c r="S92">
         <v>0.04501749490288694</v>
       </c>
-      <c r="S92">
+      <c r="T92">
         <v>0.02195547950592814</v>
       </c>
-      <c r="T92">
+      <c r="U92">
         <v>6254.553390789839</v>
       </c>
-      <c r="U92">
+      <c r="V92">
         <v>3486.45529832734</v>
       </c>
     </row>
@@ -4444,15 +4569,18 @@
         <v>6866.388733728712</v>
       </c>
       <c r="R93">
+        <v>0</v>
+      </c>
+      <c r="S93">
         <v>0.001961640809651897</v>
       </c>
-      <c r="S93">
+      <c r="T93">
         <v>0.0009951404192183229</v>
       </c>
-      <c r="T93">
+      <c r="U93">
         <v>105.7988663820767</v>
       </c>
-      <c r="U93">
+      <c r="V93">
         <v>141.4883839195763</v>
       </c>
     </row>
@@ -4513,15 +4641,18 @@
         <v>57272.46304497466</v>
       </c>
       <c r="R94">
+        <v>0</v>
+      </c>
+      <c r="S94">
         <v>0.01462471460265718</v>
       </c>
-      <c r="S94">
+      <c r="T94">
         <v>0.007772904511151228</v>
       </c>
-      <c r="T94">
+      <c r="U94">
         <v>1072.846630965207</v>
       </c>
-      <c r="U94">
+      <c r="V94">
         <v>1264.61690994371</v>
       </c>
     </row>
@@ -4582,15 +4713,18 @@
         <v>113388.3532323165</v>
       </c>
       <c r="R95">
+        <v>0</v>
+      </c>
+      <c r="S95">
         <v>0.0259047612941541</v>
       </c>
-      <c r="S95">
+      <c r="T95">
         <v>0.01339518914853143</v>
       </c>
-      <c r="T95">
+      <c r="U95">
         <v>2217.819041694451</v>
       </c>
-      <c r="U95">
+      <c r="V95">
         <v>2523.292321435117</v>
       </c>
     </row>
@@ -4651,15 +4785,18 @@
         <v>259865.7235831229</v>
       </c>
       <c r="R96">
+        <v>0</v>
+      </c>
+      <c r="S96">
         <v>0.05457543032457894</v>
       </c>
-      <c r="S96">
+      <c r="T96">
         <v>0.02803015530704517</v>
       </c>
-      <c r="T96">
+      <c r="U96">
         <v>5575.926283161257</v>
       </c>
-      <c r="U96">
+      <c r="V96">
         <v>5614.354501878082</v>
       </c>
     </row>
@@ -4720,15 +4857,18 @@
         <v>388875.5127990248</v>
       </c>
       <c r="R97">
+        <v>0</v>
+      </c>
+      <c r="S97">
         <v>0.07441804943213846</v>
       </c>
-      <c r="S97">
+      <c r="T97">
         <v>0.03785118492768021</v>
       </c>
-      <c r="T97">
+      <c r="U97">
         <v>8804.426928734993</v>
       </c>
-      <c r="U97">
+      <c r="V97">
         <v>8760.676525284971</v>
       </c>
     </row>
@@ -4789,15 +4929,18 @@
         <v>488392.4124509733</v>
       </c>
       <c r="R98">
+        <v>0</v>
+      </c>
+      <c r="S98">
         <v>0.08485510633228878</v>
       </c>
-      <c r="S98">
+      <c r="T98">
         <v>0.04290474045436292</v>
       </c>
-      <c r="T98">
+      <c r="U98">
         <v>12338.13568621884</v>
       </c>
-      <c r="U98">
+      <c r="V98">
         <v>11215.84635817243</v>
       </c>
     </row>
@@ -4858,15 +5001,18 @@
         <v>1140386.747707428</v>
       </c>
       <c r="R99">
+        <v>0.005829195638413056</v>
+      </c>
+      <c r="S99">
         <v>0.1894158404102449</v>
       </c>
-      <c r="S99">
+      <c r="T99">
         <v>0.09586136820905099</v>
       </c>
-      <c r="T99">
+      <c r="U99">
         <v>34621.70182717437</v>
       </c>
-      <c r="U99">
+      <c r="V99">
         <v>28351.34389552672</v>
       </c>
     </row>
@@ -4927,15 +5073,18 @@
         <v>539630.7040948016</v>
       </c>
       <c r="R100">
+        <v>0.04060672958947692</v>
+      </c>
+      <c r="S100">
         <v>0.1097435336932459</v>
       </c>
-      <c r="S100">
+      <c r="T100">
         <v>0.04799396686068162</v>
       </c>
-      <c r="T100">
+      <c r="U100">
         <v>15971.48692726988</v>
       </c>
-      <c r="U100">
+      <c r="V100">
         <v>14109.53964171341</v>
       </c>
     </row>
@@ -4996,15 +5145,18 @@
         <v>717254.0199252185</v>
       </c>
       <c r="R101">
+        <v>0.03809537716022157</v>
+      </c>
+      <c r="S101">
         <v>0.1295231278316404</v>
       </c>
-      <c r="S101">
+      <c r="T101">
         <v>0.060290851625477</v>
       </c>
-      <c r="T101">
+      <c r="U101">
         <v>25754.90225940232</v>
       </c>
-      <c r="U101">
+      <c r="V101">
         <v>19554.07256363844</v>
       </c>
     </row>
@@ -5065,15 +5217,18 @@
         <v>866457.7213671837</v>
       </c>
       <c r="R102">
+        <v>0.03526112128488679</v>
+      </c>
+      <c r="S102">
         <v>0.1493038961060609</v>
       </c>
-      <c r="S102">
+      <c r="T102">
         <v>0.06878972912299897</v>
       </c>
-      <c r="T102">
+      <c r="U102">
         <v>36470.67587378268</v>
       </c>
-      <c r="U102">
+      <c r="V102">
         <v>26623.45547781051</v>
       </c>
     </row>
@@ -5134,15 +5289,18 @@
         <v>945323.0708342849</v>
       </c>
       <c r="R103">
+        <v>0.02102751883702238</v>
+      </c>
+      <c r="S103">
         <v>0.1775874320583766</v>
       </c>
-      <c r="S103">
+      <c r="T103">
         <v>0.07665172649860183</v>
       </c>
-      <c r="T103">
+      <c r="U103">
         <v>44415.11879114941</v>
       </c>
-      <c r="U103">
+      <c r="V103">
         <v>29482.05288300003</v>
       </c>
     </row>
@@ -5203,15 +5361,18 @@
         <v>740766.6763984344</v>
       </c>
       <c r="R104">
+        <v>0.05549400742498291</v>
+      </c>
+      <c r="S104">
         <v>0.1431067723946153</v>
       </c>
-      <c r="S104">
+      <c r="T104">
         <v>0.05958039659656554</v>
       </c>
-      <c r="T104">
+      <c r="U104">
         <v>36337.62252390232</v>
       </c>
-      <c r="U104">
+      <c r="V104">
         <v>24176.11631396417</v>
       </c>
     </row>
@@ -5272,15 +5433,18 @@
         <v>646504.1301295699</v>
       </c>
       <c r="R105">
+        <v>0.0680503298503229</v>
+      </c>
+      <c r="S105">
         <v>0.1235424862501823</v>
       </c>
-      <c r="S105">
+      <c r="T105">
         <v>0.05425261020931529</v>
       </c>
-      <c r="T105">
+      <c r="U105">
         <v>30580.94821908279</v>
       </c>
-      <c r="U105">
+      <c r="V105">
         <v>21533.81380468671</v>
       </c>
     </row>
@@ -5341,15 +5505,18 @@
         <v>262744.9386895847</v>
       </c>
       <c r="R106">
+        <v>0.1793725156470244</v>
+      </c>
+      <c r="S106">
         <v>0.04988710187971807</v>
       </c>
-      <c r="S106">
+      <c r="T106">
         <v>0.02146054820949438</v>
       </c>
-      <c r="T106">
+      <c r="U106">
         <v>13551.12069363362</v>
       </c>
-      <c r="U106">
+      <c r="V106">
         <v>8193.406042783405</v>
       </c>
     </row>
@@ -5410,15 +5577,18 @@
         <v>106165.2669545338</v>
       </c>
       <c r="R107">
+        <v>0.1414676921636149</v>
+      </c>
+      <c r="S107">
         <v>0.019860453756475</v>
       </c>
-      <c r="S107">
+      <c r="T107">
         <v>0.008719388792811958</v>
       </c>
-      <c r="T107">
+      <c r="U107">
         <v>4855.001419509677</v>
       </c>
-      <c r="U107">
+      <c r="V107">
         <v>3229.456426580603</v>
       </c>
     </row>
@@ -5479,15 +5649,18 @@
         <v>169893.6117699225</v>
       </c>
       <c r="R108">
+        <v>0</v>
+      </c>
+      <c r="S108">
         <v>0.0305306273978112</v>
       </c>
-      <c r="S108">
+      <c r="T108">
         <v>0.01329183603749305</v>
       </c>
-      <c r="T108">
+      <c r="U108">
         <v>8561.571557414216</v>
       </c>
-      <c r="U108">
+      <c r="V108">
         <v>5784.45354285194</v>
       </c>
     </row>
@@ -5548,15 +5721,18 @@
         <v>191355.6633676433</v>
       </c>
       <c r="R109">
+        <v>0</v>
+      </c>
+      <c r="S109">
         <v>0.0284233063940974</v>
       </c>
-      <c r="S109">
+      <c r="T109">
         <v>0.01315817364995218</v>
       </c>
-      <c r="T109">
+      <c r="U109">
         <v>4906.555470965212</v>
       </c>
-      <c r="U109">
+      <c r="V109">
         <v>5446.809589277445</v>
       </c>
     </row>

</xml_diff>